<commit_message>
TAU: added:some crasy lab
</commit_message>
<xml_diff>
--- a/Г-динамика/lab1.xlsx
+++ b/Г-динамика/lab1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/diontep/workspace/6sem/Г-динамика/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14151A58-6A9C-EB4F-AED5-33F9BB04ADE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD764F4-7A2B-D14D-9DF6-5DD4A5F69891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{6257912B-16B0-234E-9101-DAE32206A608}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6257912B-16B0-234E-9101-DAE32206A608}"/>
   </bookViews>
   <sheets>
     <sheet name="Danya(4gradusa)" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>P_b вверх:</t>
   </si>
@@ -99,12 +99,6 @@
     <t>СуA: (снизу)</t>
   </si>
   <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
     <t>(инт py dy)</t>
   </si>
   <si>
@@ -131,15 +125,34 @@
   <si>
     <t>L</t>
   </si>
+  <si>
+    <t>V_inf(м/с)</t>
+  </si>
+  <si>
+    <t>v_inf(м/с)</t>
+  </si>
+  <si>
+    <t>b_inf(м)</t>
+  </si>
+  <si>
+    <t>Re</t>
+  </si>
+  <si>
+    <t>Re_inf</t>
+  </si>
+  <si>
+    <t>N дрен точек</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.00000"/>
     <numFmt numFmtId="166" formatCode="#,##0.00000000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -260,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -287,6 +300,8 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -601,33 +616,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A053EE38-C134-274D-8C02-D6F3167566FB}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="119" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="119" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" style="25"/>
     <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="4"/>
@@ -657,17 +673,17 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="1"/>
@@ -1304,17 +1320,17 @@
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
       <c r="G19" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="1"/>
@@ -2052,13 +2068,13 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="1"/>
+      <c r="C40" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="D40" s="26"/>
       <c r="E40" s="1"/>
       <c r="F40" s="2"/>
       <c r="G40" s="4"/>
@@ -2077,13 +2093,13 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="1"/>
+      <c r="C41" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="D41" s="26"/>
       <c r="E41" s="1"/>
       <c r="F41" s="2"/>
       <c r="G41" s="4"/>
@@ -2097,9 +2113,9 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="1"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="5"/>
@@ -2113,13 +2129,13 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="26">
         <v>130</v>
       </c>
-      <c r="D43" s="1"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
@@ -2133,9 +2149,9 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="1"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="5"/>
@@ -2149,9 +2165,13 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="1"/>
+      <c r="B45" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="26">
+        <v>20</v>
+      </c>
+      <c r="D45" s="26"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="5"/>
@@ -2165,9 +2185,13 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="1"/>
+      <c r="B46" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="26">
+        <v>15.06</v>
+      </c>
+      <c r="D46" s="26"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="5"/>
@@ -2181,9 +2205,16 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="1"/>
+      <c r="B47" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="D47" s="27">
+        <f>C47*1000000</f>
+        <v>200000</v>
+      </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="5"/>
@@ -2197,9 +2228,14 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="1"/>
+      <c r="B48" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="26">
+        <f>C45*D47/C46</f>
+        <v>265604.24966799468</v>
+      </c>
+      <c r="D48" s="26"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="5"/>
@@ -2210,6 +2246,13 @@
       <c r="L48" s="6"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3488,20 +3531,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF89312-12CE-EE45-AF69-A373FDF7D160}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="119" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView topLeftCell="A19" zoomScale="119" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="25"/>
     <col min="10" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B1" s="1"/>
       <c r="C1" s="3"/>
       <c r="D1" s="1"/>
@@ -3534,17 +3580,17 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="1"/>
@@ -4180,17 +4226,17 @@
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
       <c r="G19" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="1"/>
@@ -4911,11 +4957,11 @@
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="A39" s="26"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="2"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -4927,15 +4973,15 @@
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="C40" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
       <c r="F40" s="2"/>
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
@@ -4955,15 +5001,15 @@
       <c r="N40" s="1"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1" t="s">
+      <c r="A41" s="26"/>
+      <c r="B41" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+      <c r="C41" s="26">
+        <v>0.12</v>
+      </c>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
       <c r="F41" s="2"/>
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
@@ -4978,11 +5024,11 @@
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
       <c r="F42" s="1"/>
       <c r="G42" s="5"/>
       <c r="H42" s="4"/>
@@ -4994,15 +5040,15 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
+      <c r="A43" s="26"/>
+      <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="26">
         <v>117</v>
       </c>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
       <c r="F43" s="1"/>
       <c r="G43" s="5"/>
       <c r="H43" s="4"/>
@@ -5014,11 +5060,11 @@
       <c r="N43" s="1"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
       <c r="F44" s="1"/>
       <c r="G44" s="5"/>
       <c r="H44" s="4"/>
@@ -5030,11 +5076,15 @@
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="26">
+        <v>20</v>
+      </c>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
       <c r="F45" s="1"/>
       <c r="G45" s="5"/>
       <c r="H45" s="4"/>
@@ -5046,11 +5096,15 @@
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="26">
+        <v>15.06</v>
+      </c>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
       <c r="F46" s="1"/>
       <c r="G46" s="5"/>
       <c r="H46" s="4"/>
@@ -5062,11 +5116,18 @@
       <c r="N46" s="1"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="D47" s="27">
+        <f>C47*1000000</f>
+        <v>200000</v>
+      </c>
+      <c r="E47" s="26"/>
       <c r="F47" s="1"/>
       <c r="G47" s="5"/>
       <c r="H47" s="4"/>
@@ -5078,11 +5139,16 @@
       <c r="N47" s="1"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="26">
+        <f>C45*D47/C46</f>
+        <v>265604.24966799468</v>
+      </c>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
       <c r="F48" s="1"/>
       <c r="G48" s="5"/>
       <c r="H48" s="4"/>
@@ -5093,6 +5159,57 @@
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
     </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="26"/>
+      <c r="B49" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="26"/>
+      <c r="B50" s="26"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="26"/>
+      <c r="B51" s="26"/>
+      <c r="C51" s="26"/>
+      <c r="D51" s="26"/>
+      <c r="E51" s="26"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="26"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="26"/>
+      <c r="D52" s="26"/>
+      <c r="E52" s="26"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="26"/>
+      <c r="B53" s="26"/>
+      <c r="C53" s="26"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="26"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="26"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="26"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="26"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="D55" s="26"/>
+      <c r="E55" s="26"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>